<commit_message>
Se modifico la interfaz del menu principal. Ademas se agregaron restriciones de agregacion, modificacion y de pago a base de abonos de Bordadora para proteger la integracion de datos de la base de datos
</commit_message>
<xml_diff>
--- a/InventarioCompleto.xlsx
+++ b/InventarioCompleto.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -76,163 +76,169 @@
     <t>saldo</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
   <si>
     <t>1000.0</t>
   </si>
   <si>
-    <t>192222.0</t>
-  </si>
-  <si>
-    <t>niguno</t>
+    <t>1010.0</t>
+  </si>
+  <si>
+    <t>tumadrexd</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>yu</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>111.0</t>
+  </si>
+  <si>
+    <t>Gilberto</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>2000.0</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>1110.0</t>
+  </si>
+  <si>
+    <t>111110.0</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
   <si>
     <t>2020</t>
   </si>
   <si>
-    <t>noses</t>
-  </si>
-  <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>jajaja</t>
+    <t>no</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Yamaha1</t>
+  </si>
+  <si>
+    <t>11110.0</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>Maquinas</t>
+  </si>
+  <si>
+    <t>galga_men</t>
+  </si>
+  <si>
+    <t>galga_mayor</t>
+  </si>
+  <si>
+    <t>nivel</t>
+  </si>
+  <si>
+    <t>cantida</t>
+  </si>
+  <si>
+    <t>tamano</t>
+  </si>
+  <si>
+    <t>etiqueta</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>maquinas</t>
+  </si>
+  <si>
+    <t>unidad</t>
+  </si>
+  <si>
+    <t>HOLA</t>
+  </si>
+  <si>
+    <t>galaga</t>
+  </si>
+  <si>
+    <t>aguna</t>
+  </si>
+  <si>
+    <t>mi casa</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>sasz</t>
+  </si>
+  <si>
+    <t>dssd</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>ggg</t>
+  </si>
+  <si>
+    <t>yhh</t>
+  </si>
+  <si>
+    <t>hhh</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>234.0</t>
   </si>
   <si>
     <t>nose</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3455.0</t>
-  </si>
-  <si>
-    <t>escutia</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>1010.0</t>
-  </si>
-  <si>
-    <t>tumadrexd</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>ds</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>juan</t>
-  </si>
-  <si>
-    <t>yu</t>
-  </si>
-  <si>
-    <t>11110.0</t>
-  </si>
-  <si>
-    <t>Gilberto</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>Maquinas</t>
-  </si>
-  <si>
-    <t>galga_men</t>
-  </si>
-  <si>
-    <t>galga_mayor</t>
-  </si>
-  <si>
-    <t>nivel</t>
-  </si>
-  <si>
-    <t>cantida</t>
-  </si>
-  <si>
-    <t>tamano</t>
-  </si>
-  <si>
-    <t>etiqueta</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>maquinas</t>
-  </si>
-  <si>
-    <t>unidad</t>
-  </si>
-  <si>
-    <t>HOLA</t>
-  </si>
-  <si>
-    <t>galaga</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>aguna</t>
-  </si>
-  <si>
-    <t>mi casa</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>sasz</t>
-  </si>
-  <si>
-    <t>dssd</t>
-  </si>
-  <si>
-    <t>20.0</t>
-  </si>
-  <si>
-    <t>ggg</t>
-  </si>
-  <si>
-    <t>yhh</t>
-  </si>
-  <si>
-    <t>hhh</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>234.0</t>
   </si>
   <si>
     <t>soodod</t>
@@ -432,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>3</v>
@@ -441,25 +447,25 @@
         <v>7</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s" s="0">
         <v>6</v>
       </c>
       <c r="K1" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -480,10 +486,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>3</v>
@@ -492,25 +498,25 @@
         <v>7</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K1" t="s" s="0">
         <v>6</v>
       </c>
       <c r="L1" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +526,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -613,40 +619,81 @@
         <v>30</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="G3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>38</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>27</v>
       </c>
       <c r="L3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="M3" t="s" s="0">
+      <c r="G4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>40</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -667,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>3</v>
@@ -676,25 +723,25 @@
         <v>7</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s" s="0">
         <v>6</v>
       </c>
       <c r="K1" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -715,10 +762,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>3</v>
@@ -727,25 +774,25 @@
         <v>7</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K1" t="s" s="0">
         <v>6</v>
       </c>
       <c r="L1" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -801,104 +848,104 @@
         <v>27</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>59</v>
-      </c>
       <c r="I3" t="s" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -957,84 +1004,84 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>27</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>79</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>58</v>
-      </c>
       <c r="L3" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1055,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>3</v>
@@ -1064,25 +1111,25 @@
         <v>7</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s" s="0">
         <v>6</v>
       </c>
       <c r="K1" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1103,10 +1150,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>3</v>
@@ -1115,25 +1162,25 @@
         <v>7</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K1" t="s" s="0">
         <v>6</v>
       </c>
       <c r="L1" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>